<commit_message>
Anforderungsspezifikation Aktualisiert. Bis Sonntag wird noch das fachliche Datenmodell hinzugefügt.
</commit_message>
<xml_diff>
--- a/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Benutzeranforderungen.xlsx
+++ b/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Benutzeranforderungen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="52">
   <si>
     <t>Art</t>
   </si>
@@ -408,6 +408,91 @@
   <si>
     <t>6/Client-Init
 8/Server-Spiel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8/Server-Spiel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Version: 1.1</t>
+    </r>
+  </si>
+  <si>
+    <t>Länder die einem bestimmten 
+Spieler nicht gehören, werden nicht
+"ausgegraut", sondern in den Farben
+des entsprechenden Besitzers ange-
+zeigt</t>
+  </si>
+  <si>
+    <t>Spart Ressourcen,
+da jedem Client die
+gleiche Spielkarte
+angezeigt wird</t>
+  </si>
+  <si>
+    <t>Bosin
+(10.10.2018)</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5/Server-GUI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Version: 1.1</t>
+    </r>
+  </si>
+  <si>
+    <t>Erste Anzeige sind zwei Buttons zur
+Auswahl: neues Spiel und Spiel
+laden</t>
+  </si>
+  <si>
+    <t>Die Unterscheidung
+ist nötig, da nur 
+bei einem neuen 
+Spiel die Spieler-
+anzahl festgelegt
+werden muss.</t>
+  </si>
+  <si>
+    <t>Kunde
+(10.10.2018)</t>
   </si>
 </sst>
 </file>
@@ -504,7 +589,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -542,8 +627,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,8 +667,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="41">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -598,6 +690,8 @@
     <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -616,6 +710,8 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -894,7 +990,7 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:E34"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1282,15 +1378,31 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+    <row r="19" spans="1:10" ht="105" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
@@ -1522,15 +1634,31 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+    <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>

</xml_diff>